<commit_message>
added more columns because of ui issues out of screen.
</commit_message>
<xml_diff>
--- a/fcat_1.0/src/test/resources/Catalogs/Excel.xlsx
+++ b/fcat_1.0/src/test/resources/Catalogs/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="47200" windowHeight="27340" tabRatio="500"/>
+    <workbookView xWindow="10160" yWindow="3780" windowWidth="47200" windowHeight="27340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>mf</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nones</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -398,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -416,8 +428,17 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -428,7 +449,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
new file with more columns and data.
</commit_message>
<xml_diff>
--- a/fcat_1.0/src/test/resources/Catalogs/Excel.xlsx
+++ b/fcat_1.0/src/test/resources/Catalogs/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="3780" windowWidth="47200" windowHeight="27340" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="47200" windowHeight="27340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -448,6 +448,15 @@
       <c r="C2">
         <v>123</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
@@ -461,6 +470,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>